<commit_message>
Site updated: 2020-07-04 00:06:22
</commit_message>
<xml_diff>
--- a/data/totaltime.xlsx
+++ b/data/totaltime.xlsx
@@ -1,19 +1,50 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mambawang\themes\next\source\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1EE15F-AE58-4DC6-8E2A-DE9AFB54E5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="mySheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>mins</t>
+  </si>
+  <si>
+    <t>secs</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -50,6 +81,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,48 +413,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>hours</v>
-      </c>
-      <c r="B1" t="str">
-        <v>mins</v>
-      </c>
-      <c r="C1" t="str">
-        <v>secs</v>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>hours</v>
-      </c>
-      <c r="B2" t="str">
-        <v>mins</v>
-      </c>
-      <c r="C2" t="str">
-        <v>secs</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>127</v>
-      </c>
-      <c r="B3" t="str">
-        <v>31</v>
-      </c>
-      <c r="C3" t="str">
-        <v>21</v>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError sqref="A1:C2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>